<commit_message>
update the README and the first SOTA
</commit_message>
<xml_diff>
--- a/SOTA/blink.xlsx
+++ b/SOTA/blink.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\useful\PDPTW\SOTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9EE30A-A3D9-4DFC-8218-F409C6768C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B33252-EC18-441B-B950-9327722A5047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="46">
   <si>
     <t xml:space="preserve"> Inst   </t>
   </si>
@@ -136,13 +136,52 @@
   </si>
   <si>
     <t xml:space="preserve"> poa-n100-7 </t>
+  </si>
+  <si>
+    <t>SISRs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vehicles</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gap_c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gap_v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="0.000%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,10 +197,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FFCF8E6D"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -181,16 +221,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,15 +511,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:AD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0.01</v>
       </c>
@@ -500,7 +542,7 @@
         <v>5</v>
       </c>
       <c r="H1">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -520,9 +562,50 @@
       <c r="N1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="O1">
+        <v>0.05</v>
+      </c>
+      <c r="P1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1">
+        <v>0.1</v>
+      </c>
+      <c r="X1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -559,9 +642,44 @@
       <c r="N2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" t="s">
+        <v>11</v>
+      </c>
+      <c r="X2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -580,27 +698,78 @@
       <c r="G3">
         <v>6</v>
       </c>
+      <c r="H3">
+        <f>(D3-G3)/G3</f>
+        <v>0</v>
+      </c>
       <c r="I3" t="s">
         <v>12</v>
       </c>
       <c r="J3">
+        <v>757</v>
+      </c>
+      <c r="K3">
+        <v>6</v>
+      </c>
+      <c r="L3">
+        <v>23.35</v>
+      </c>
+      <c r="M3">
+        <v>3.27</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <f>(K3-N3)/N3</f>
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3">
         <v>756</v>
       </c>
-      <c r="K3">
-        <v>6</v>
-      </c>
-      <c r="L3">
+      <c r="R3">
+        <v>6</v>
+      </c>
+      <c r="S3">
         <v>19.79</v>
       </c>
-      <c r="M3">
+      <c r="T3">
         <v>3.14</v>
       </c>
-      <c r="N3">
-        <v>6</v>
-      </c>
-      <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="U3">
+        <v>6</v>
+      </c>
+      <c r="V3">
+        <f>(R3-U3)/U3</f>
+        <v>0</v>
+      </c>
+      <c r="X3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y3">
+        <v>748</v>
+      </c>
+      <c r="Z3">
+        <v>6</v>
+      </c>
+      <c r="AA3">
+        <v>19.8</v>
+      </c>
+      <c r="AB3">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AC3">
+        <v>6</v>
+      </c>
+      <c r="AD3">
+        <f>(Z3-AC3)/AC3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -619,27 +788,78 @@
       <c r="G4">
         <v>5</v>
       </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H30" si="0">(D4-G4)/G4</f>
+        <v>0</v>
+      </c>
       <c r="I4" t="s">
         <v>13</v>
       </c>
       <c r="J4">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="L4">
-        <v>16.510000000000002</v>
+        <v>19.53</v>
       </c>
       <c r="M4">
-        <v>6.32</v>
+        <v>5.24</v>
       </c>
       <c r="N4">
         <v>5</v>
       </c>
-      <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="O4">
+        <f t="shared" ref="O4:O27" si="1">(K4-N4)/N4</f>
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4">
+        <v>589</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <v>16.510000000000002</v>
+      </c>
+      <c r="T4">
+        <v>6.32</v>
+      </c>
+      <c r="U4">
+        <v>5</v>
+      </c>
+      <c r="V4">
+        <f t="shared" ref="V4:V27" si="2">(R4-U4)/U4</f>
+        <v>0</v>
+      </c>
+      <c r="X4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y4">
+        <v>582</v>
+      </c>
+      <c r="Z4">
+        <v>5</v>
+      </c>
+      <c r="AA4">
+        <v>17.47</v>
+      </c>
+      <c r="AB4">
+        <v>5.05</v>
+      </c>
+      <c r="AC4">
+        <v>5</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" ref="AD4:AD27" si="3">(Z4-AC4)/AC4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -658,27 +878,78 @@
       <c r="G5">
         <v>6</v>
       </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I5" t="s">
         <v>14</v>
       </c>
       <c r="J5">
+        <v>755</v>
+      </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <v>10.8</v>
+      </c>
+      <c r="M5">
+        <v>1.21</v>
+      </c>
+      <c r="N5">
+        <v>6</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5">
         <v>750</v>
       </c>
-      <c r="K5">
-        <v>6</v>
-      </c>
-      <c r="L5">
+      <c r="R5">
+        <v>6</v>
+      </c>
+      <c r="S5">
         <v>11.03</v>
       </c>
-      <c r="M5">
+      <c r="T5">
         <v>0.54</v>
       </c>
-      <c r="N5">
-        <v>6</v>
-      </c>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="U5">
+        <v>6</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y5">
+        <v>756</v>
+      </c>
+      <c r="Z5">
+        <v>6</v>
+      </c>
+      <c r="AA5">
+        <v>19.96</v>
+      </c>
+      <c r="AB5">
+        <v>1.34</v>
+      </c>
+      <c r="AC5">
+        <v>6</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -697,27 +968,78 @@
       <c r="G6">
         <v>12</v>
       </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
       <c r="I6" t="s">
         <v>15</v>
       </c>
       <c r="J6">
-        <v>1190</v>
+        <v>1160</v>
       </c>
       <c r="K6">
         <v>14</v>
       </c>
       <c r="L6">
-        <v>16.489999999999998</v>
+        <v>26.52</v>
       </c>
       <c r="M6">
-        <v>3.12</v>
+        <v>0.52</v>
       </c>
       <c r="N6">
         <v>12</v>
       </c>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q6">
+        <v>1190</v>
+      </c>
+      <c r="R6">
+        <v>14</v>
+      </c>
+      <c r="S6">
+        <v>16.489999999999998</v>
+      </c>
+      <c r="T6">
+        <v>3.12</v>
+      </c>
+      <c r="U6">
+        <v>12</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="X6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y6">
+        <v>1194</v>
+      </c>
+      <c r="Z6">
+        <v>13</v>
+      </c>
+      <c r="AA6">
+        <v>33.32</v>
+      </c>
+      <c r="AB6">
+        <v>3.47</v>
+      </c>
+      <c r="AC6">
+        <v>12</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -736,27 +1058,78 @@
       <c r="G7">
         <v>6</v>
       </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I7" t="s">
         <v>16</v>
       </c>
       <c r="J7">
+        <v>882</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>12.72</v>
+      </c>
+      <c r="M7">
+        <v>5.25</v>
+      </c>
+      <c r="N7">
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7">
         <v>885</v>
       </c>
-      <c r="K7">
-        <v>6</v>
-      </c>
-      <c r="L7">
+      <c r="R7">
+        <v>6</v>
+      </c>
+      <c r="S7">
         <v>9.34</v>
       </c>
-      <c r="M7">
+      <c r="T7">
         <v>5.61</v>
       </c>
-      <c r="N7">
-        <v>6</v>
-      </c>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="U7">
+        <v>6</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y7">
+        <v>908</v>
+      </c>
+      <c r="Z7">
+        <v>6</v>
+      </c>
+      <c r="AA7">
+        <v>19.2</v>
+      </c>
+      <c r="AB7">
+        <v>8.35</v>
+      </c>
+      <c r="AC7">
+        <v>6</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -775,27 +1148,78 @@
       <c r="G8">
         <v>3</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
       <c r="I8" t="s">
         <v>17</v>
       </c>
       <c r="J8">
-        <v>773</v>
+        <v>777</v>
       </c>
       <c r="K8">
         <v>4</v>
       </c>
       <c r="L8">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="M8">
+        <v>-1.4</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="P8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q8">
+        <v>773</v>
+      </c>
+      <c r="R8">
+        <v>4</v>
+      </c>
+      <c r="S8">
         <v>12.14</v>
       </c>
-      <c r="M8">
+      <c r="T8">
         <v>-1.9</v>
       </c>
-      <c r="N8">
-        <v>3</v>
-      </c>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="U8">
+        <v>3</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="X8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y8">
+        <v>798</v>
+      </c>
+      <c r="Z8">
+        <v>4</v>
+      </c>
+      <c r="AA8">
+        <v>15.68</v>
+      </c>
+      <c r="AB8">
+        <v>1.27</v>
+      </c>
+      <c r="AC8">
+        <v>3</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -814,6 +1238,10 @@
       <c r="G9">
         <v>13</v>
       </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
       <c r="I9" t="s">
         <v>18</v>
       </c>
@@ -821,10 +1249,10 @@
         <v>1884</v>
       </c>
       <c r="K9">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L9">
-        <v>20.53</v>
+        <v>20.88</v>
       </c>
       <c r="M9">
         <v>1.45</v>
@@ -832,9 +1260,56 @@
       <c r="N9">
         <v>13</v>
       </c>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="P9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9">
+        <v>1884</v>
+      </c>
+      <c r="R9">
+        <v>15</v>
+      </c>
+      <c r="S9">
+        <v>20.53</v>
+      </c>
+      <c r="T9">
+        <v>1.45</v>
+      </c>
+      <c r="U9">
+        <v>13</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="2"/>
+        <v>0.15384615384615385</v>
+      </c>
+      <c r="X9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y9">
+        <v>1888</v>
+      </c>
+      <c r="Z9">
+        <v>14</v>
+      </c>
+      <c r="AA9">
+        <v>34.9</v>
+      </c>
+      <c r="AB9">
+        <v>1.67</v>
+      </c>
+      <c r="AC9">
+        <v>13</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="3"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -853,27 +1328,78 @@
       <c r="G10">
         <v>6</v>
       </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
       <c r="I10" t="s">
         <v>19</v>
       </c>
       <c r="J10">
-        <v>1554</v>
+        <v>1557</v>
       </c>
       <c r="K10">
         <v>7</v>
       </c>
       <c r="L10">
+        <v>10.6</v>
+      </c>
+      <c r="M10">
+        <v>4.43</v>
+      </c>
+      <c r="N10">
+        <v>6</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10">
+        <v>1554</v>
+      </c>
+      <c r="R10">
+        <v>7</v>
+      </c>
+      <c r="S10">
         <v>12.32</v>
       </c>
-      <c r="M10">
+      <c r="T10">
         <v>4.22</v>
       </c>
-      <c r="N10">
-        <v>6</v>
-      </c>
-      <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="U10">
+        <v>6</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="X10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y10">
+        <v>1549</v>
+      </c>
+      <c r="Z10">
+        <v>7</v>
+      </c>
+      <c r="AA10">
+        <v>21.5</v>
+      </c>
+      <c r="AB10">
+        <v>3.89</v>
+      </c>
+      <c r="AC10">
+        <v>6</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="3"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -892,27 +1418,78 @@
       <c r="G11">
         <v>3</v>
       </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I11" t="s">
         <v>20</v>
       </c>
       <c r="J11">
+        <v>731</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <v>5.52</v>
+      </c>
+      <c r="M11">
+        <v>2.52</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q11">
         <v>723</v>
       </c>
-      <c r="K11">
-        <v>3</v>
-      </c>
-      <c r="L11">
+      <c r="R11">
+        <v>3</v>
+      </c>
+      <c r="S11">
         <v>6.43</v>
       </c>
-      <c r="M11">
+      <c r="T11">
         <v>1.4</v>
       </c>
-      <c r="N11">
-        <v>3</v>
-      </c>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="U11">
+        <v>3</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X11" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y11">
+        <v>723</v>
+      </c>
+      <c r="Z11">
+        <v>3</v>
+      </c>
+      <c r="AA11">
+        <v>10.86</v>
+      </c>
+      <c r="AB11">
+        <v>1.4</v>
+      </c>
+      <c r="AC11">
+        <v>3</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>21</v>
       </c>
@@ -931,27 +1508,78 @@
       <c r="G12">
         <v>3</v>
       </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I12" t="s">
         <v>21</v>
       </c>
       <c r="J12">
+        <v>496</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>6.58</v>
+      </c>
+      <c r="M12">
+        <v>0.41</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12">
         <v>495</v>
       </c>
-      <c r="K12">
-        <v>3</v>
-      </c>
-      <c r="L12">
+      <c r="R12">
+        <v>3</v>
+      </c>
+      <c r="S12">
         <v>7.14</v>
       </c>
-      <c r="M12">
+      <c r="T12">
         <v>0.2</v>
       </c>
-      <c r="N12">
-        <v>3</v>
-      </c>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="U12">
+        <v>3</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X12" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y12">
+        <v>497</v>
+      </c>
+      <c r="Z12">
+        <v>3</v>
+      </c>
+      <c r="AA12">
+        <v>13.46</v>
+      </c>
+      <c r="AB12">
+        <v>0.61</v>
+      </c>
+      <c r="AC12">
+        <v>3</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>22</v>
       </c>
@@ -970,27 +1598,78 @@
       <c r="G13">
         <v>5</v>
       </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I13" t="s">
         <v>22</v>
       </c>
       <c r="J13">
-        <v>968</v>
+        <v>955</v>
       </c>
       <c r="K13">
         <v>5</v>
       </c>
       <c r="L13">
-        <v>10.24</v>
+        <v>8.66</v>
       </c>
       <c r="M13">
-        <v>2.54</v>
+        <v>1.17</v>
       </c>
       <c r="N13">
         <v>5</v>
       </c>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13">
+        <v>968</v>
+      </c>
+      <c r="R13">
+        <v>5</v>
+      </c>
+      <c r="S13">
+        <v>10.24</v>
+      </c>
+      <c r="T13">
+        <v>2.54</v>
+      </c>
+      <c r="U13">
+        <v>5</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y13">
+        <v>953</v>
+      </c>
+      <c r="Z13">
+        <v>5</v>
+      </c>
+      <c r="AA13">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="AB13">
+        <v>0.95</v>
+      </c>
+      <c r="AC13">
+        <v>5</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>23</v>
       </c>
@@ -1009,27 +1688,78 @@
       <c r="G14">
         <v>14</v>
       </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
       <c r="I14" t="s">
         <v>23</v>
       </c>
       <c r="J14">
-        <v>2111</v>
+        <v>2077</v>
       </c>
       <c r="K14">
         <v>15</v>
       </c>
       <c r="L14">
-        <v>21.1</v>
+        <v>18.14</v>
       </c>
       <c r="M14">
-        <v>-1.68</v>
+        <v>-3.26</v>
       </c>
       <c r="N14">
         <v>14</v>
       </c>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="O14">
+        <f t="shared" si="1"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="P14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q14">
+        <v>2111</v>
+      </c>
+      <c r="R14">
+        <v>15</v>
+      </c>
+      <c r="S14">
+        <v>21.1</v>
+      </c>
+      <c r="T14">
+        <v>-1.68</v>
+      </c>
+      <c r="U14">
+        <v>14</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="2"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="X14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y14">
+        <v>2154</v>
+      </c>
+      <c r="Z14">
+        <v>15</v>
+      </c>
+      <c r="AA14">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="AB14">
+        <v>0.33</v>
+      </c>
+      <c r="AC14">
+        <v>14</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="3"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -1048,27 +1778,78 @@
       <c r="G15">
         <v>7</v>
       </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I15" t="s">
         <v>24</v>
       </c>
       <c r="J15">
-        <v>1905</v>
+        <v>1926</v>
       </c>
       <c r="K15">
         <v>8</v>
       </c>
       <c r="L15">
-        <v>13.55</v>
+        <v>11.19</v>
       </c>
       <c r="M15">
-        <v>-1.55</v>
+        <v>-0.47</v>
       </c>
       <c r="N15">
         <v>7</v>
       </c>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="O15">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="P15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q15">
+        <v>1905</v>
+      </c>
+      <c r="R15">
+        <v>8</v>
+      </c>
+      <c r="S15">
+        <v>13.55</v>
+      </c>
+      <c r="T15">
+        <v>-1.55</v>
+      </c>
+      <c r="U15">
+        <v>7</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="2"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="X15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y15">
+        <v>1976</v>
+      </c>
+      <c r="Z15">
+        <v>8</v>
+      </c>
+      <c r="AA15">
+        <v>23.05</v>
+      </c>
+      <c r="AB15">
+        <v>2.12</v>
+      </c>
+      <c r="AC15">
+        <v>7</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="3"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>25</v>
       </c>
@@ -1087,27 +1868,78 @@
       <c r="G16">
         <v>6</v>
       </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I16" t="s">
         <v>25</v>
       </c>
       <c r="J16">
+        <v>651</v>
+      </c>
+      <c r="K16">
+        <v>6</v>
+      </c>
+      <c r="L16">
+        <v>10.36</v>
+      </c>
+      <c r="M16">
+        <v>2.68</v>
+      </c>
+      <c r="N16">
+        <v>6</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q16">
         <v>646</v>
       </c>
-      <c r="K16">
-        <v>6</v>
-      </c>
-      <c r="L16">
+      <c r="R16">
+        <v>6</v>
+      </c>
+      <c r="S16">
         <v>12.63</v>
       </c>
-      <c r="M16">
+      <c r="T16">
         <v>1.89</v>
       </c>
-      <c r="N16">
-        <v>6</v>
-      </c>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="2:15">
+      <c r="U16">
+        <v>6</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X16" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y16">
+        <v>648</v>
+      </c>
+      <c r="Z16">
+        <v>6</v>
+      </c>
+      <c r="AA16">
+        <v>21</v>
+      </c>
+      <c r="AB16">
+        <v>2.21</v>
+      </c>
+      <c r="AC16">
+        <v>6</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>26</v>
       </c>
@@ -1126,27 +1958,78 @@
       <c r="G17">
         <v>4</v>
       </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I17" t="s">
         <v>26</v>
       </c>
       <c r="J17">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="K17">
         <v>4</v>
       </c>
       <c r="L17">
-        <v>10.65</v>
+        <v>9.09</v>
       </c>
       <c r="M17">
-        <v>1.24</v>
+        <v>1.41</v>
       </c>
       <c r="N17">
         <v>4</v>
       </c>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="2:15">
+      <c r="O17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q17">
+        <v>574</v>
+      </c>
+      <c r="R17">
+        <v>4</v>
+      </c>
+      <c r="S17">
+        <v>10.65</v>
+      </c>
+      <c r="T17">
+        <v>1.24</v>
+      </c>
+      <c r="U17">
+        <v>4</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X17" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y17">
+        <v>572</v>
+      </c>
+      <c r="Z17">
+        <v>4</v>
+      </c>
+      <c r="AA17">
+        <v>17.73</v>
+      </c>
+      <c r="AB17">
+        <v>0.88</v>
+      </c>
+      <c r="AC17">
+        <v>4</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>27</v>
       </c>
@@ -1165,27 +2048,78 @@
       <c r="G18">
         <v>3</v>
       </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
       <c r="I18" t="s">
         <v>27</v>
       </c>
       <c r="J18">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="K18">
         <v>4</v>
       </c>
       <c r="L18">
+        <v>9.18</v>
+      </c>
+      <c r="M18">
+        <v>-6.1</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="P18" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q18">
+        <v>461</v>
+      </c>
+      <c r="R18">
+        <v>4</v>
+      </c>
+      <c r="S18">
         <v>10.6</v>
       </c>
-      <c r="M18">
+      <c r="T18">
         <v>-6.3</v>
       </c>
-      <c r="N18">
-        <v>3</v>
-      </c>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="2:15">
+      <c r="U18">
+        <v>3</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="X18" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y18">
+        <v>486</v>
+      </c>
+      <c r="Z18">
+        <v>4</v>
+      </c>
+      <c r="AA18">
+        <v>18.62</v>
+      </c>
+      <c r="AB18">
+        <v>-1.22</v>
+      </c>
+      <c r="AC18">
+        <v>3</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>28</v>
       </c>
@@ -1204,27 +2138,78 @@
       <c r="G19">
         <v>2</v>
       </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
       <c r="I19" t="s">
         <v>28</v>
       </c>
       <c r="J19">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="K19">
         <v>3</v>
       </c>
       <c r="L19">
-        <v>9.81</v>
+        <v>8.43</v>
       </c>
       <c r="M19">
-        <v>3.92</v>
+        <v>3.55</v>
       </c>
       <c r="N19">
         <v>2</v>
       </c>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="2:15">
+      <c r="O19">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="P19" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q19">
+        <v>556</v>
+      </c>
+      <c r="R19">
+        <v>3</v>
+      </c>
+      <c r="S19">
+        <v>9.81</v>
+      </c>
+      <c r="T19">
+        <v>3.92</v>
+      </c>
+      <c r="U19">
+        <v>2</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="X19" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y19">
+        <v>555</v>
+      </c>
+      <c r="Z19">
+        <v>3</v>
+      </c>
+      <c r="AA19">
+        <v>16.690000000000001</v>
+      </c>
+      <c r="AB19">
+        <v>3.74</v>
+      </c>
+      <c r="AC19">
+        <v>2</v>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>29</v>
       </c>
@@ -1243,27 +2228,78 @@
       <c r="G20">
         <v>2</v>
       </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
       <c r="I20" t="s">
         <v>29</v>
       </c>
       <c r="J20">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="K20">
         <v>3</v>
       </c>
       <c r="L20">
-        <v>10.44</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="M20">
-        <v>-0.45</v>
+        <v>-1.64</v>
       </c>
       <c r="N20">
         <v>2</v>
       </c>
-      <c r="O20" s="1"/>
-    </row>
-    <row r="21" spans="2:15">
+      <c r="O20">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="P20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q20">
+        <v>668</v>
+      </c>
+      <c r="R20">
+        <v>3</v>
+      </c>
+      <c r="S20">
+        <v>10.44</v>
+      </c>
+      <c r="T20">
+        <v>-0.45</v>
+      </c>
+      <c r="U20">
+        <v>2</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="X20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y20">
+        <v>677</v>
+      </c>
+      <c r="Z20">
+        <v>3</v>
+      </c>
+      <c r="AA20">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="AB20">
+        <v>0.89</v>
+      </c>
+      <c r="AC20">
+        <v>2</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>30</v>
       </c>
@@ -1282,27 +2318,78 @@
       <c r="G21">
         <v>12</v>
       </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="I21" t="s">
         <v>30</v>
       </c>
       <c r="J21">
-        <v>1627</v>
+        <v>1632</v>
       </c>
       <c r="K21">
         <v>13</v>
       </c>
       <c r="L21">
-        <v>18.760000000000002</v>
+        <v>16</v>
       </c>
       <c r="M21">
-        <v>2.39</v>
+        <v>2.71</v>
       </c>
       <c r="N21">
         <v>12</v>
       </c>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="2:15">
+      <c r="O21">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="P21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q21">
+        <v>1627</v>
+      </c>
+      <c r="R21">
+        <v>13</v>
+      </c>
+      <c r="S21">
+        <v>18.760000000000002</v>
+      </c>
+      <c r="T21">
+        <v>2.39</v>
+      </c>
+      <c r="U21">
+        <v>12</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="2"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="X21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y21">
+        <v>1658</v>
+      </c>
+      <c r="Z21">
+        <v>13</v>
+      </c>
+      <c r="AA21">
+        <v>33.58</v>
+      </c>
+      <c r="AB21">
+        <v>4.34</v>
+      </c>
+      <c r="AC21">
+        <v>12</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>31</v>
       </c>
@@ -1321,27 +2408,78 @@
       <c r="G22">
         <v>15</v>
       </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
       <c r="I22" t="s">
         <v>31</v>
       </c>
       <c r="J22">
-        <v>1592</v>
+        <v>1579</v>
       </c>
       <c r="K22">
         <v>16</v>
       </c>
       <c r="L22">
-        <v>22.56</v>
+        <v>18.91</v>
       </c>
       <c r="M22">
-        <v>3.44</v>
+        <v>2.6</v>
       </c>
       <c r="N22">
         <v>15</v>
       </c>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="2:15">
+      <c r="O22">
+        <f t="shared" si="1"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="P22" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q22">
+        <v>1592</v>
+      </c>
+      <c r="R22">
+        <v>16</v>
+      </c>
+      <c r="S22">
+        <v>22.56</v>
+      </c>
+      <c r="T22">
+        <v>3.44</v>
+      </c>
+      <c r="U22">
+        <v>15</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="2"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="X22" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y22">
+        <v>1581</v>
+      </c>
+      <c r="Z22">
+        <v>16</v>
+      </c>
+      <c r="AA22">
+        <v>38.81</v>
+      </c>
+      <c r="AB22">
+        <v>2.73</v>
+      </c>
+      <c r="AC22">
+        <v>15</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="3"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>32</v>
       </c>
@@ -1360,27 +2498,78 @@
       <c r="G23">
         <v>10</v>
       </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="I23" t="s">
         <v>32</v>
       </c>
       <c r="J23">
-        <v>1306</v>
+        <v>1275</v>
       </c>
       <c r="K23">
         <v>12</v>
       </c>
       <c r="L23">
-        <v>31.41</v>
+        <v>15.42</v>
       </c>
       <c r="M23">
-        <v>0.38</v>
+        <v>-2</v>
       </c>
       <c r="N23">
         <v>10</v>
       </c>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="2:15">
+      <c r="O23">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="P23" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q23">
+        <v>1306</v>
+      </c>
+      <c r="R23">
+        <v>12</v>
+      </c>
+      <c r="S23">
+        <v>31.41</v>
+      </c>
+      <c r="T23">
+        <v>0.38</v>
+      </c>
+      <c r="U23">
+        <v>10</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="X23" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y23">
+        <v>1324</v>
+      </c>
+      <c r="Z23">
+        <v>12</v>
+      </c>
+      <c r="AA23">
+        <v>31.42</v>
+      </c>
+      <c r="AB23">
+        <v>1.77</v>
+      </c>
+      <c r="AC23">
+        <v>10</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>33</v>
       </c>
@@ -1399,27 +2588,78 @@
       <c r="G24">
         <v>7</v>
       </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>0.2857142857142857</v>
+      </c>
       <c r="I24" t="s">
         <v>33</v>
       </c>
       <c r="J24">
-        <v>1623</v>
+        <v>1568</v>
       </c>
       <c r="K24">
         <v>9</v>
       </c>
       <c r="L24">
-        <v>18.22</v>
+        <v>12.32</v>
       </c>
       <c r="M24">
-        <v>-2.7</v>
+        <v>-6</v>
       </c>
       <c r="N24">
         <v>7</v>
       </c>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="2:15">
+      <c r="O24">
+        <f t="shared" si="1"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="P24" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q24">
+        <v>1623</v>
+      </c>
+      <c r="R24">
+        <v>9</v>
+      </c>
+      <c r="S24">
+        <v>18.22</v>
+      </c>
+      <c r="T24">
+        <v>-2.7</v>
+      </c>
+      <c r="U24">
+        <v>7</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="2"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="X24" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y24">
+        <v>1561</v>
+      </c>
+      <c r="Z24">
+        <v>9</v>
+      </c>
+      <c r="AA24">
+        <v>24.86</v>
+      </c>
+      <c r="AB24">
+        <v>-6.42</v>
+      </c>
+      <c r="AC24">
+        <v>7</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="3"/>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>34</v>
       </c>
@@ -1438,27 +2678,78 @@
       <c r="G25">
         <v>6</v>
       </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I25" t="s">
         <v>34</v>
       </c>
       <c r="J25">
+        <v>628</v>
+      </c>
+      <c r="K25">
+        <v>6</v>
+      </c>
+      <c r="L25">
+        <v>9.52</v>
+      </c>
+      <c r="M25">
+        <v>0.64</v>
+      </c>
+      <c r="N25">
+        <v>6</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P25" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q25">
         <v>645</v>
       </c>
-      <c r="K25">
-        <v>6</v>
-      </c>
-      <c r="L25">
+      <c r="R25">
+        <v>6</v>
+      </c>
+      <c r="S25">
         <v>16.48</v>
       </c>
-      <c r="M25">
+      <c r="T25">
         <v>3.37</v>
       </c>
-      <c r="N25">
-        <v>6</v>
-      </c>
-      <c r="O25" s="1"/>
-    </row>
-    <row r="26" spans="2:15">
+      <c r="U25">
+        <v>6</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X25" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y25">
+        <v>635</v>
+      </c>
+      <c r="Z25">
+        <v>6</v>
+      </c>
+      <c r="AA25">
+        <v>19.23</v>
+      </c>
+      <c r="AB25">
+        <v>1.76</v>
+      </c>
+      <c r="AC25">
+        <v>6</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>35</v>
       </c>
@@ -1477,27 +2768,78 @@
       <c r="G26">
         <v>3</v>
       </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I26" t="s">
         <v>35</v>
       </c>
       <c r="J26">
+        <v>570</v>
+      </c>
+      <c r="K26">
+        <v>3</v>
+      </c>
+      <c r="L26">
+        <v>5.57</v>
+      </c>
+      <c r="M26">
+        <v>1.42</v>
+      </c>
+      <c r="N26">
+        <v>3</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P26" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q26">
         <v>575</v>
       </c>
-      <c r="K26">
-        <v>3</v>
-      </c>
-      <c r="L26">
+      <c r="R26">
+        <v>3</v>
+      </c>
+      <c r="S26">
         <v>9.3000000000000007</v>
       </c>
-      <c r="M26">
+      <c r="T26">
         <v>2.31</v>
       </c>
-      <c r="N26">
-        <v>3</v>
-      </c>
-      <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="2:15">
+      <c r="U26">
+        <v>3</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X26" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y26">
+        <v>578</v>
+      </c>
+      <c r="Z26">
+        <v>3</v>
+      </c>
+      <c r="AA26">
+        <v>8.36</v>
+      </c>
+      <c r="AB26">
+        <v>2.85</v>
+      </c>
+      <c r="AC26">
+        <v>3</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>36</v>
       </c>
@@ -1516,27 +2858,78 @@
       <c r="G27">
         <v>5</v>
       </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="I27" t="s">
         <v>36</v>
       </c>
       <c r="J27">
-        <v>744</v>
+        <v>733</v>
       </c>
       <c r="K27">
         <v>6</v>
       </c>
       <c r="L27">
-        <v>13.78</v>
+        <v>9.56</v>
       </c>
       <c r="M27">
-        <v>-4.49</v>
+        <v>-5.91</v>
       </c>
       <c r="N27">
         <v>5</v>
       </c>
-      <c r="O27" s="1"/>
-    </row>
-    <row r="28" spans="2:15">
+      <c r="O27">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="P27" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q27">
+        <v>744</v>
+      </c>
+      <c r="R27">
+        <v>6</v>
+      </c>
+      <c r="S27">
+        <v>13.78</v>
+      </c>
+      <c r="T27">
+        <v>-4.49</v>
+      </c>
+      <c r="U27">
+        <v>5</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="X27" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y27">
+        <v>752</v>
+      </c>
+      <c r="Z27">
+        <v>6</v>
+      </c>
+      <c r="AA27">
+        <v>20.27</v>
+      </c>
+      <c r="AB27">
+        <v>-3.47</v>
+      </c>
+      <c r="AC27">
+        <v>5</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C28">
         <f>AVERAGE(C3:C27)</f>
         <v>1021.88</v>
@@ -1557,28 +2950,84 @@
         <f>AVERAGE(G3:G27)</f>
         <v>6.56</v>
       </c>
+      <c r="H28">
+        <f>AVERAGE(H3:H27)</f>
+        <v>0.11936263736263739</v>
+      </c>
       <c r="J28">
         <f>AVERAGE(J3:J27)</f>
-        <v>1024</v>
+        <v>1017.08</v>
       </c>
       <c r="K28">
         <f>AVERAGE(K3:K27)</f>
-        <v>7.28</v>
+        <v>7.24</v>
       </c>
       <c r="L28">
         <f>AVERAGE(L3:L27)</f>
-        <v>14.450000000000003</v>
+        <v>12.658000000000001</v>
       </c>
       <c r="M28">
         <f>AVERAGE(M3:M27)</f>
-        <v>1.1363999999999999</v>
+        <v>0.54800000000000026</v>
       </c>
       <c r="N28">
         <f>AVERAGE(N3:N27)</f>
         <v>6.56</v>
       </c>
-    </row>
-    <row r="29" spans="2:15">
+      <c r="O28">
+        <f>AVERAGE(O3:O27)</f>
+        <v>0.12507692307692309</v>
+      </c>
+      <c r="Q28">
+        <f>AVERAGE(Q3:Q27)</f>
+        <v>1024</v>
+      </c>
+      <c r="R28">
+        <f>AVERAGE(R3:R27)</f>
+        <v>7.28</v>
+      </c>
+      <c r="S28">
+        <f>AVERAGE(S3:S27)</f>
+        <v>14.450000000000003</v>
+      </c>
+      <c r="T28">
+        <f>AVERAGE(T3:T27)</f>
+        <v>1.1363999999999999</v>
+      </c>
+      <c r="U28">
+        <f>AVERAGE(U3:U27)</f>
+        <v>6.56</v>
+      </c>
+      <c r="V28">
+        <f>AVERAGE(V3:V27)</f>
+        <v>0.12815384615384617</v>
+      </c>
+      <c r="Y28">
+        <f>AVERAGE(Y3:Y27)</f>
+        <v>1030.1199999999999</v>
+      </c>
+      <c r="Z28">
+        <f>AVERAGE(Z3:Z27)</f>
+        <v>7.2</v>
+      </c>
+      <c r="AA28">
+        <f>AVERAGE(AA3:AA27)</f>
+        <v>22.056000000000004</v>
+      </c>
+      <c r="AB28">
+        <f>AVERAGE(AB3:AB27)</f>
+        <v>1.7024000000000001</v>
+      </c>
+      <c r="AC28">
+        <f>AVERAGE(AC3:AC27)</f>
+        <v>6.56</v>
+      </c>
+      <c r="AD28">
+        <f>AVERAGE(AD3:AD27)</f>
+        <v>0.12174358974358977</v>
+      </c>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C29">
         <f>SUM(C3:C27)</f>
         <v>25547</v>
@@ -1601,24 +3050,251 @@
       </c>
       <c r="J29">
         <f>SUM(J3:J27)</f>
-        <v>25600</v>
+        <v>25427</v>
       </c>
       <c r="K29">
         <f>SUM(K3:K27)</f>
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L29">
         <f>SUM(L3:L27)</f>
-        <v>361.25000000000006</v>
+        <v>316.45000000000005</v>
       </c>
       <c r="M29">
         <f>SUM(M3:M27)</f>
-        <v>28.409999999999997</v>
+        <v>13.700000000000006</v>
       </c>
       <c r="N29">
         <f>SUM(N3:N27)</f>
         <v>164</v>
       </c>
+      <c r="Q29">
+        <f>SUM(Q3:Q27)</f>
+        <v>25600</v>
+      </c>
+      <c r="R29">
+        <f>SUM(R3:R27)</f>
+        <v>182</v>
+      </c>
+      <c r="S29">
+        <f>SUM(S3:S27)</f>
+        <v>361.25000000000006</v>
+      </c>
+      <c r="T29">
+        <f>SUM(T3:T27)</f>
+        <v>28.409999999999997</v>
+      </c>
+      <c r="U29">
+        <f>SUM(U3:U27)</f>
+        <v>164</v>
+      </c>
+      <c r="Y29">
+        <f>SUM(Y3:Y27)</f>
+        <v>25753</v>
+      </c>
+      <c r="Z29">
+        <f>SUM(Z3:Z27)</f>
+        <v>180</v>
+      </c>
+      <c r="AA29">
+        <f>SUM(AA3:AA27)</f>
+        <v>551.40000000000009</v>
+      </c>
+      <c r="AB29">
+        <f>SUM(AB3:AB27)</f>
+        <v>42.56</v>
+      </c>
+      <c r="AC29">
+        <f>SUM(AC3:AC27)</f>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>25355</v>
+      </c>
+      <c r="D30">
+        <v>164</v>
+      </c>
+      <c r="F30">
+        <f>(C29-C30)/C30</f>
+        <v>7.5724709130349042E-3</v>
+      </c>
+      <c r="G30">
+        <f>(D29-D30)/D30</f>
+        <v>9.7560975609756101E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>37</v>
+      </c>
+      <c r="J33" t="s">
+        <v>42</v>
+      </c>
+      <c r="K33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L33" t="s">
+        <v>44</v>
+      </c>
+      <c r="M33" t="s">
+        <v>45</v>
+      </c>
+      <c r="P33">
+        <v>0.01</v>
+      </c>
+      <c r="Q33">
+        <v>0.03</v>
+      </c>
+      <c r="R33">
+        <v>0.05</v>
+      </c>
+      <c r="S33">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>38</v>
+      </c>
+      <c r="I34">
+        <v>25547</v>
+      </c>
+      <c r="J34">
+        <v>25388</v>
+      </c>
+      <c r="K34">
+        <v>25579</v>
+      </c>
+      <c r="L34">
+        <v>25445</v>
+      </c>
+      <c r="M34">
+        <v>25588</v>
+      </c>
+      <c r="O34" t="s">
+        <v>38</v>
+      </c>
+      <c r="P34">
+        <v>25547</v>
+      </c>
+      <c r="Q34">
+        <v>25427</v>
+      </c>
+      <c r="R34">
+        <v>25600</v>
+      </c>
+      <c r="S34">
+        <v>25753</v>
+      </c>
+    </row>
+    <row r="35" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>39</v>
+      </c>
+      <c r="I35">
+        <v>180</v>
+      </c>
+      <c r="J35">
+        <v>164</v>
+      </c>
+      <c r="K35">
+        <v>165</v>
+      </c>
+      <c r="L35">
+        <v>164</v>
+      </c>
+      <c r="M35">
+        <v>165</v>
+      </c>
+      <c r="O35" t="s">
+        <v>39</v>
+      </c>
+      <c r="P35">
+        <v>180</v>
+      </c>
+      <c r="Q35">
+        <v>181</v>
+      </c>
+      <c r="R35">
+        <v>182</v>
+      </c>
+      <c r="S35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>40</v>
+      </c>
+      <c r="I36" s="1">
+        <v>8.7600000000000004E-3</v>
+      </c>
+      <c r="J36" s="1">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="K36" s="1">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="L36" s="1">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="M36" s="1">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="O36" t="s">
+        <v>40</v>
+      </c>
+      <c r="P36" s="1">
+        <v>8.7600000000000004E-3</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>5.4799999999999996E-3</v>
+      </c>
+      <c r="R36" s="1">
+        <v>1.136E-2</v>
+      </c>
+      <c r="S36" s="1">
+        <v>1.7024000000000001E-2</v>
+      </c>
+      <c r="T36" s="1"/>
+    </row>
+    <row r="37" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>41</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0.11935999999999999</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="L37" s="1">
+        <v>0</v>
+      </c>
+      <c r="M37" s="1">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="O37" t="s">
+        <v>41</v>
+      </c>
+      <c r="P37" s="1">
+        <v>0.11935999999999999</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>0.12508</v>
+      </c>
+      <c r="R37" s="1">
+        <v>0.12814999999999999</v>
+      </c>
+      <c r="S37" s="1">
+        <v>0.12174</v>
+      </c>
+      <c r="T37" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>